<commit_message>
CMA Compliance template update
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS/CMA/Data/CMA Compliance Template v0.2.xlsx
+++ b/Projects/CCBOTTLERSUS/CMA/Data/CMA Compliance Template v0.2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="118">
   <si>
     <t>KPI name</t>
   </si>
@@ -252,7 +252,7 @@
     <t>POWERADE</t>
   </si>
   <si>
-    <t>size</t>
+    <t>att3</t>
   </si>
   <si>
     <t>32</t>
@@ -303,7 +303,7 @@
     <t>GLACEAU VITAMIN WATER</t>
   </si>
   <si>
-    <t>Client Subcategory Name</t>
+    <t>sub_category</t>
   </si>
   <si>
     <t>Enhanced</t>
@@ -328,6 +328,12 @@
   </si>
   <si>
     <t>Monster Energy Muscle Peanut Butter Cup Energy Shakes 15oz 4pack,Monster Energy Muscle Vanilla Energy Shakes,Monster Energy Muscle Monster Vanilla 16oz,Monster Energy Muscle Monster Chocolate 16oz,MONSTER Muscle Monster Chocolate 12/15oz,MONSTER Muscle Monster Vanilla 12/15oz</t>
+  </si>
+  <si>
+    <t>SHELF STABLE PROTEIN</t>
+  </si>
+  <si>
+    <t>SHELF STABLE DAIRY</t>
   </si>
   <si>
     <t>ZICO COCONUT WATER</t>
@@ -440,7 +446,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -508,6 +514,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
@@ -523,7 +536,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -552,12 +565,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0000CC"/>
-        <bgColor rgb="FF0000FF"/>
       </patternFill>
     </fill>
     <fill>
@@ -764,15 +771,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -784,7 +791,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -804,7 +811,7 @@
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000CC"/>
+      <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
@@ -868,18 +875,18 @@
   </sheetPr>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E11" activeCellId="1" sqref="D6 E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.3846153846154"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.7085020242915"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.5627530364373"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.2064777327935"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.21052631578947"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.8502024291498"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="34.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
@@ -1228,13 +1235,13 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="1" sqref="D6 B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="4" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="44.3481781376518"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="44.9919028340081"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="4" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="1013" min="4" style="4" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1022" min="1014" style="5" width="9.10526315789474"/>
@@ -1281,24 +1288,24 @@
   </sheetPr>
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.3846153846154"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.2753036437247"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="28.3846153846154"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="36.5263157894737"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="37.17004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
@@ -1428,7 +1435,7 @@
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
     </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -1748,7 +1755,7 @@
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
     </row>
-    <row r="20" customFormat="false" ht="243.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="210.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="26" t="s">
         <v>31</v>
       </c>
@@ -1764,8 +1771,12 @@
       <c r="E20" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
+      <c r="F20" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G20" s="29" t="s">
+        <v>82</v>
+      </c>
       <c r="H20" s="21"/>
       <c r="I20" s="21"/>
     </row>
@@ -1781,8 +1792,12 @@
       </c>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
+      <c r="F21" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G21" s="29" t="s">
+        <v>83</v>
+      </c>
       <c r="H21" s="21"/>
       <c r="I21" s="21"/>
     </row>
@@ -1794,7 +1809,7 @@
         <v>51</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D22" s="23"/>
       <c r="E22" s="23"/>
@@ -1808,7 +1823,7 @@
         <v>73</v>
       </c>
       <c r="I22" s="16" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1830,7 +1845,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="1" sqref="D6 E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1845,19 +1860,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1865,16 +1880,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>50</v>
@@ -1899,29 +1914,29 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="1" sqref="D6 D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.0283400809717"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.4574898785425"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1929,10 +1944,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1943,7 +1958,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1954,7 +1969,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1976,7 +1991,7 @@
         <v>16</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1987,7 +2002,7 @@
         <v>18</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1998,7 +2013,7 @@
         <v>19</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2009,7 +2024,7 @@
         <v>20</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2020,7 +2035,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2031,7 +2046,7 @@
         <v>22</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2042,7 +2057,7 @@
         <v>23</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2050,10 +2065,10 @@
         <v>24</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D13" s="32" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2064,7 +2079,7 @@
         <v>25</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2075,7 +2090,7 @@
         <v>26</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2086,18 +2101,18 @@
         <v>27</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2108,7 +2123,7 @@
         <v>29</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2119,7 +2134,7 @@
         <v>30</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2130,7 +2145,7 @@
         <v>31</v>
       </c>
       <c r="D20" s="33" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2141,7 +2156,7 @@
         <v>32</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2152,7 +2167,7 @@
         <v>33</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CMA Compliance targets were added
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS/CMA/Data/CMA Compliance Template v0.2.xlsx
+++ b/Projects/CCBOTTLERSUS/CMA/Data/CMA Compliance Template v0.2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="120">
   <si>
     <t>KPI name</t>
   </si>
@@ -252,7 +252,7 @@
     <t>POWERADE</t>
   </si>
   <si>
-    <t>att3</t>
+    <t>size</t>
   </si>
   <si>
     <t>32</t>
@@ -360,15 +360,24 @@
     <t>UNITED</t>
   </si>
   <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>lafayette</t>
+    <t>Baton Rouge Red</t>
+  </si>
+  <si>
+    <t>Baton Rouge</t>
   </si>
   <si>
     <t>Convenience</t>
   </si>
   <si>
+    <t>Monster JAVA/Café</t>
+  </si>
+  <si>
+    <t>Core Power/Monster Muscle</t>
+  </si>
+  <si>
+    <t>Baton Rouge Black</t>
+  </si>
+  <si>
     <t>Confirmed by Steve:</t>
   </si>
   <si>
@@ -418,9 +427,6 @@
   </si>
   <si>
     <t> Enhanced Water</t>
-  </si>
-  <si>
-    <t>Monster JAVA/Café</t>
   </si>
   <si>
     <t> RTD Coffee ?  Correct.</t>
@@ -442,11 +448,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="0%"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -517,6 +524,12 @@
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -654,7 +667,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -775,11 +788,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -791,7 +820,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -876,17 +905,17 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="1" sqref="D6 E11"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.1376518218623"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.2064777327935"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.8502024291498"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.21052631578947"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="34.4939271255061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="34.919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
@@ -1235,13 +1264,13 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="1" sqref="D6 B8"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="4" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="44.9919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="45.8461538461538"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="4" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="1013" min="4" style="4" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1022" min="1014" style="5" width="9.10526315789474"/>
@@ -1288,24 +1317,24 @@
   </sheetPr>
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B10" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.2753036437247"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.6761133603239"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="37.17004048583"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="37.7044534412955"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
@@ -1485,7 +1514,7 @@
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
     </row>
-    <row r="8" customFormat="false" ht="77.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="76.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
@@ -1508,7 +1537,7 @@
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
     </row>
-    <row r="9" customFormat="false" ht="108.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
@@ -1554,7 +1583,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
     </row>
-    <row r="11" customFormat="false" ht="155" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="136.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
@@ -1842,20 +1871,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="1" sqref="D6 E13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="9.21052631578947"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.17813765182186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.9433198380567"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.8056680161943"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -1875,14 +1907,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="30" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="31" t="s">
         <v>92</v>
       </c>
       <c r="D2" s="0" t="s">
@@ -1891,8 +1923,828 @@
       <c r="E2" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <v>50</v>
+      <c r="F2" s="32" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" s="32" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="32" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="32" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" s="32" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" s="32" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="32" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9" s="32" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="32" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F11" s="32" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" s="32" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" s="32" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F14" s="32" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" s="32" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="32" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17" s="32" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" s="32" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" s="32" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" s="32" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F21" s="32" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" s="32" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F23" s="32" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" s="32" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" s="32" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26" s="32" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27" s="32" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C28" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" s="32" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F29" s="32" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F30" s="32" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F31" s="32" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F32" s="32" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F33" s="32" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F34" s="32" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F35" s="32" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F36" s="32" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F37" s="32" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F38" s="32" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F39" s="32" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F40" s="32" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F41" s="32" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F42" s="32" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F43" s="32" t="n">
+        <v>0.6</v>
       </c>
     </row>
   </sheetData>
@@ -1913,73 +2765,73 @@
   </sheetPr>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="1" sqref="D6 D11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="27.8502024291498"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.4574898785425"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.9919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="D1" s="31" t="s">
         <v>98</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>100</v>
+      <c r="C2" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="32" t="s">
-        <v>101</v>
+      <c r="D3" s="36" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="32" t="s">
-        <v>102</v>
+      <c r="D4" s="36" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="36" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1987,187 +2839,187 @@
       <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="32" t="s">
-        <v>103</v>
+      <c r="D6" s="36" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="32" t="s">
-        <v>104</v>
+      <c r="D7" s="36" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="32" t="s">
-        <v>104</v>
+      <c r="D8" s="36" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="33" t="s">
-        <v>105</v>
+      <c r="D9" s="37" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="32" t="s">
-        <v>106</v>
+      <c r="D10" s="36" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="33" t="s">
-        <v>107</v>
+      <c r="D11" s="37" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="32" t="s">
-        <v>106</v>
+      <c r="D12" s="36" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="D13" s="32" t="s">
-        <v>109</v>
+      <c r="C13" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" s="36" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="34" t="s">
-        <v>110</v>
+      <c r="D14" s="38" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="32" t="s">
-        <v>111</v>
+      <c r="D15" s="36" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="32" t="s">
-        <v>111</v>
+      <c r="D16" s="36" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C17" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="D17" s="33" t="s">
-        <v>113</v>
+        <v>95</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" s="37" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="32" t="s">
-        <v>114</v>
+      <c r="D18" s="36" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="32" t="s">
-        <v>114</v>
+      <c r="D19" s="36" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="32" t="s">
+      <c r="C20" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="33" t="s">
-        <v>115</v>
+      <c r="D20" s="37" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="33" t="s">
-        <v>116</v>
+      <c r="D21" s="37" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="C22" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="34" t="s">
-        <v>117</v>
+      <c r="D22" s="38" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CMA Compliance level1 score
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS/CMA/Data/CMA Compliance Template v0.2.xlsx
+++ b/Projects/CCBOTTLERSUS/CMA/Data/CMA Compliance Template v0.2.xlsx
@@ -360,13 +360,13 @@
     <t>UNITED</t>
   </si>
   <si>
-    <t>Baton Rouge Red</t>
+    <t>Red</t>
   </si>
   <si>
     <t>Baton Rouge</t>
   </si>
   <si>
-    <t>Convenience</t>
+    <t>CR&amp;LT</t>
   </si>
   <si>
     <t>Monster JAVA/Café</t>
@@ -905,17 +905,17 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="1" sqref="C17:C22 E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.3522267206478"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.17004048583"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.21052631578947"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="34.919028340081"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.1336032388664"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
@@ -1264,13 +1264,13 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="1" sqref="C17:C22 B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="4" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="45.8461538461538"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="46.2753036437247"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="4" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="1013" min="4" style="4" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1022" min="1014" style="5" width="9.10526315789474"/>
@@ -1318,23 +1318,23 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B10" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
+      <selection pane="topLeft" activeCell="I22" activeCellId="1" sqref="C17:C22 I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.919028340081"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.2388663967611"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="37.919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
@@ -1874,16 +1874,16 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.21052631578947"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.17813765182186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.4939271255061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.9433198380567"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.8056680161943"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.2834008097166"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.0647773279352"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
@@ -2766,14 +2766,14 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
+      <selection pane="topLeft" activeCell="B37" activeCellId="1" sqref="C17:C22 B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.9919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.3117408906883"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>